<commit_message>
SM Review agenda list and MOM archived.
</commit_message>
<xml_diff>
--- a/PEG-22-23_MINMET.xlsx
+++ b/PEG-22-23_MINMET.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="122">
   <si>
     <t>Instructions for Use</t>
   </si>
@@ -1222,6 +1222,112 @@
   </si>
   <si>
     <t>Jalaj</t>
+  </si>
+  <si>
+    <t>MBR (Q-2) Review</t>
+  </si>
+  <si>
+    <t>Tarun Gupta, Jalaj Mathur</t>
+  </si>
+  <si>
+    <t>Jalaj conveyed that last time indetified action item "Line rejection percentage goal need to change to 2.5% in Business KPI page of Einframe" already done.</t>
+  </si>
+  <si>
+    <t>MBR Review : Schedule Variance</t>
+  </si>
+  <si>
+    <t>Action Item :
+1. After completion of current on going projects, review and revise the schedule variance goal.
+2. Recruitments of experienced persons in middle level.</t>
+  </si>
+  <si>
+    <t>After completion of current on going projects, review and revise the schedule variance goal.</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>Recruitments of experienced persons in middle level.</t>
+  </si>
+  <si>
+    <t>Tarun Gupta</t>
+  </si>
+  <si>
+    <t>MBR Review : Line Rejection Ratio</t>
+  </si>
+  <si>
+    <t>Jalaj conveyed that overall the average figure is 2.77 % which is near to our goal i.e. 2.5%. This is due to our testing and validation team efforts in projects as well as components validation. In May &amp; August month this ratio went some high say 3.5%. This high failure ratio was expected because engineering sample trial lot occured in this duartion.
+Tarun asked what component that was ? Jalaj conveyed that Chint make AC MCB 10A. This sample approved for trial lot previously so it is expected that it can be happen. But in future such type of electro mechanical samples parallely check in R&amp;D as well as Quality (Haridwar), so that the probability of trial lot failure reduced by some numbers. Also planned to make BOM review checklist in QMS, so that these rejected items can not make part of further models BOMs.
+Tarun convinenced and told that keep in touch with production and quality regarding this.</t>
+  </si>
+  <si>
+    <t>Action Item :
+1. Make BOM review checklist.</t>
+  </si>
+  <si>
+    <t>Make BOM review checklist.</t>
+  </si>
+  <si>
+    <t>MBR Review : Product Quality</t>
+  </si>
+  <si>
+    <t>Action Item :
+1. Explore dashboard of Incidents to monitor and control.</t>
+  </si>
+  <si>
+    <t>Jalaj conveyed that as already discussed the low line rejection ration is result of review effectiveness, testing and validation efficiency. The defects filtered during these stages. Although some improvement suggested to team that make habit for self review also to reduce the number of defects.
+Tarun asked how project managers monitor their defect density in whole project life cycle ? Jalaj conveyed and gave demo of EinFrame Incident management report for all defects in particular project. Tarun suggested that one dashboard type can be implement for these incidents, as EinFrame do for actions items / project tasks. Jalaj ensured to Tarun that he will explore the same with development team.</t>
+  </si>
+  <si>
+    <t>Explore dashboard of Incidents to monitor and control.</t>
+  </si>
+  <si>
+    <t>MBR Review : Support Functions</t>
+  </si>
+  <si>
+    <t>Jalaj conveyed that in total 6 Projects considered to collect data for schedule variance and their analysis, out of them 2 NOS are complete i.e. GGE295 &amp; GGE300. And remaining 4 NOS are on going in different different stages / phases. For completed project average schedule variance was 18.6% in positive side, although that is under limit, but far away from goal. This is due to the release related activities that were extended by one week.
+For on going projects the same trend is observing that schedule variance coming in positive side say 6% -13 % in recent completed milestone and in currently on going activities / tasks.
+So overall trend of schedule variance is always positive side near to 10%.
+Tarun asked what is our goal for schedule variance ? Jalaj conveyed that goal is 0.  Tarun called Mr. Sobhag &amp; Mr. Syoji (Project managers) and asked why we are higher side in schedule variance, we should try to recue this numbers.
+Tarun asked why not we take realastic goal to see this trends ?
+Jalaj agreed to take some relastic goals, but suggested that for more accurate goal, we should wait for currently running projects completion. After that we can set more relastic goal may be like 10% or 12% etc.
+Tarun convinenced but told that another aspect of that team take it by granted and may be variances will go more than 20%. So we should think more on that and explore backup plan also for this. Jalaj told that one thing we can do it relatively fast that recruit some experience persons in middle level also so that team enhancement can occur, as in last some months some experienced employes left the organization. In one project (GGS151) the project manager suffered with this happening, his 2 experienced team members left with short notice, so his plan was effected by this, as damage control he re-assigned some other less experienced team members, but overall his project suffers. Tarun ensured that in next recruitment drive he will focused on this, and already 2 new experienced person almost finalized, who will join within in a month.</t>
+  </si>
+  <si>
+    <t>Jalaj conveyed the performance of support fuctions like PEG, PQA and OT.
+PEG : The one major and one minor version of QMS released in last 6 months duration with coverage of Project management. As Benchmark Appraisal scheduled in Nov.22 first week, so one major version is expected after that to address appraisal’s findings. Tarun convinenced with that.
+PQA : Jalaj conveyed that after seen audit reports the same picture as discussed in schedule variance section, product quality section came.  So we'll continue with that. Although to make pool of auditor PQA head Ms. Shweta Agarwal already included project managers in audit of other project managers's projects to enhance the process adherence.
+OT : Jalaj conveyed that although coverage of trainings are OK, but overall work not as per expectation. PEG already talked to Training coordinator (Ms. Girija) regarding this and asked to improve this. It is proposed that as Senior Management you should also talked to her.</t>
+  </si>
+  <si>
+    <t>Action Item :
+1. Talk to Training coordinator to speed up activities as per plan.</t>
+  </si>
+  <si>
+    <t>Talk to Training coordinator to speed up activities as per plan.</t>
+  </si>
+  <si>
+    <t>Tarun asked what are the issues if any in stakeholders invloment. Jalaj told that as suggested internal informal review on going time to time.</t>
+  </si>
+  <si>
+    <t>Benchmark Appraisal</t>
+  </si>
+  <si>
+    <t>Tarun asked about the preparation of upcoming event i.e. Benchmark Appraisal. Jalaj convyed that :
+1. The benchmark appraisal scheduled from 1st Nov. to 9th Nov.22
+2. Logistics related tasks like train ticket booking an hote room booking done. Only need to align the pick and drop facility for Mr. Amir Khan
+3. Sampling of projects by CMMI institute already done, there are 5 projects which are sampled.
+4. ARR already done by Mr. Amir Khan (LA).</t>
+  </si>
+  <si>
+    <t>Action Item :
+1. Pick and drop facility arrangement for LA.</t>
+  </si>
+  <si>
+    <t>Pick and drop facility arrangement for LA.</t>
+  </si>
+  <si>
+    <t>13-Oct-22;  16.05 to 16.30 PM</t>
   </si>
 </sst>
 </file>
@@ -1474,7 +1580,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1488,87 +1594,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1580,6 +1614,99 @@
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1606,7 +1733,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1625,8 +1752,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:F6" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A4:F6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:F11" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A4:F11"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Sr No." dataDxfId="5"/>
     <tableColumn id="2" name="Action Item" dataDxfId="4"/>
@@ -2284,348 +2411,430 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E49"/>
+  <dimension ref="A2:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="8" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="70.7109375" style="8" customWidth="1"/>
-    <col min="4" max="4" width="29" style="8" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="8" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" width="4.7109375" style="30" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="108.28515625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" style="5" customWidth="1"/>
+    <col min="5" max="6" width="9.140625" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="33" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="15" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="13" t="s">
+      <c r="A6" s="34"/>
+      <c r="B6" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="11"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="16"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="10" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="21" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="23" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="25" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="25" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
+      <c r="A13" s="36"/>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="27" t="s">
+      <c r="D14" s="8" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="28">
+      <c r="A15" s="38">
         <v>1</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="19"/>
-    </row>
-    <row r="16" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
-      <c r="B16" s="30" t="s">
+      <c r="C15" s="11"/>
+      <c r="D15" s="21"/>
+    </row>
+    <row r="16" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="39">
+        <v>2</v>
+      </c>
+      <c r="B16" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D16" s="34" t="s">
+      <c r="D16" s="10" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
-      <c r="B17" s="28" t="s">
+    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="38">
+        <v>3</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="35" t="s">
+      <c r="C17" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="D17" s="19"/>
-    </row>
-    <row r="18" spans="1:4" ht="135" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
-      <c r="B18" s="32" t="s">
+      <c r="D17" s="21"/>
+    </row>
+    <row r="18" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A18" s="40">
+        <v>4</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="C18" s="36" t="s">
+      <c r="C18" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="D18" s="33"/>
-    </row>
-    <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="28"/>
-      <c r="B19" s="28" t="s">
+      <c r="D18" s="29"/>
+    </row>
+    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="41">
+        <v>5</v>
+      </c>
+      <c r="B19" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="D19" s="19"/>
+      <c r="D19" s="42"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="13" t="s">
+      <c r="A22" s="34"/>
+      <c r="B22" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="14"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="18"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="17"/>
+      <c r="C24" s="10" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="19"/>
+      <c r="C25" s="21" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="C26" s="21"/>
+      <c r="C26" s="23" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="23"/>
+      <c r="C27" s="25" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="C28" s="23"/>
+      <c r="C28" s="25"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="25"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="26" t="s">
+      <c r="A29" s="36"/>
+    </row>
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B30" s="26" t="s">
+      <c r="B30" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="27" t="s">
+      <c r="D30" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="28">
+    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="38">
         <v>1</v>
       </c>
-      <c r="B31" s="29" t="s">
+      <c r="B31" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="28"/>
-      <c r="D31" s="19"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
-      <c r="B32" s="30"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="17"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="28"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="19"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="32"/>
-      <c r="B34" s="32"/>
-      <c r="C34" s="32"/>
-      <c r="D34" s="33"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="12"/>
-      <c r="B37" s="13" t="s">
+      <c r="C31" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D31" s="21"/>
+    </row>
+    <row r="32" spans="1:4" ht="300" x14ac:dyDescent="0.25">
+      <c r="A32" s="39">
+        <v>2</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A33" s="38">
+        <v>3</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A34" s="40">
+        <v>4</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D34" s="29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A35" s="41">
+        <v>5</v>
+      </c>
+      <c r="B35" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D35" s="21" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="43">
+        <v>6</v>
+      </c>
+      <c r="B36" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="D36" s="29"/>
+    </row>
+    <row r="37" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A37" s="41">
+        <v>7</v>
+      </c>
+      <c r="B37" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="C37" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D37" s="42" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="34"/>
+      <c r="B40" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="14"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="16" t="s">
+      <c r="C40" s="17"/>
+      <c r="D40" s="18"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="44"/>
+      <c r="C41" s="44"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C39" s="17"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="18" t="s">
+      <c r="C42" s="10"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="19"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="20" t="s">
+      <c r="C43" s="21"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="C41" s="21"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="22" t="s">
+      <c r="C44" s="23"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="C42" s="23"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="24" t="s">
+      <c r="C45" s="25"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="C43" s="23"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="25"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="26" t="s">
+      <c r="C46" s="25"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="36"/>
+    </row>
+    <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B45" s="26" t="s">
+      <c r="B48" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="C45" s="26" t="s">
+      <c r="C48" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D45" s="27" t="s">
+      <c r="D48" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="28">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="38">
         <v>1</v>
       </c>
-      <c r="B46" s="29" t="s">
+      <c r="B49" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="28"/>
-      <c r="D46" s="19"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="30"/>
-      <c r="B47" s="30"/>
-      <c r="C47" s="30"/>
-      <c r="D47" s="17"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="28"/>
-      <c r="B48" s="28"/>
-      <c r="C48" s="28"/>
-      <c r="D48" s="19"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="32"/>
-      <c r="B49" s="32"/>
-      <c r="C49" s="32"/>
-      <c r="D49" s="33"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="21"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="39"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="10"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="38"/>
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="21"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="40"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B41:C41"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B15" location="'Action Items'!A1" display="Pending action items"/>
     <hyperlink ref="B31" location="'Action Items'!A1" display="Pending action items"/>
-    <hyperlink ref="B46" location="'Action Items'!A1" display="Pending action items"/>
+    <hyperlink ref="B49" location="'Action Items'!A1" display="Pending action items"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2637,25 +2846,27 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="32"/>
+    <col min="2" max="2" width="21.5703125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="30" t="s">
         <v>60</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -2676,19 +2887,19 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="30">
         <v>1</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C5" s="37">
+      <c r="C5" s="13">
         <v>44813</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E5" s="37">
+      <c r="E5" s="13">
         <v>44813</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -2696,64 +2907,122 @@
       </c>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+    <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="31">
         <v>2</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
+      <c r="B6" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="13">
+        <v>44880</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>100</v>
+      </c>
       <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+      <c r="F6" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="30">
+        <v>3</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="13">
+        <v>44880</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>100</v>
+      </c>
       <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="F7" s="5" t="s">
+        <v>102</v>
+      </c>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="30">
+        <v>4</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="13">
+        <v>44880</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>100</v>
+      </c>
       <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="F8" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="30">
+        <v>5</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="13">
+        <v>44880</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>100</v>
+      </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="F9" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="30">
+        <v>6</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C10" s="13">
+        <v>44849</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>100</v>
+      </c>
       <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+      <c r="F10" s="5" t="s">
+        <v>102</v>
+      </c>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="30">
+        <v>7</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" s="13">
+        <v>44865</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>100</v>
+      </c>
       <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="F11" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
+      <c r="A12" s="30"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -2762,7 +3031,7 @@
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
+      <c r="A13" s="30"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -2771,7 +3040,7 @@
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
+      <c r="A14" s="30"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -2780,7 +3049,7 @@
       <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
+      <c r="A15" s="30"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -2789,7 +3058,7 @@
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
+      <c r="A16" s="30"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -2798,7 +3067,7 @@
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
+      <c r="A17" s="30"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -2807,7 +3076,7 @@
       <c r="G17" s="5"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -2816,7 +3085,7 @@
       <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
+      <c r="A19" s="30"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -2825,7 +3094,7 @@
       <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
+      <c r="A20" s="30"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -2834,7 +3103,7 @@
       <c r="G20" s="5"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
+      <c r="A21" s="30"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -2843,7 +3112,7 @@
       <c r="G21" s="5"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
+      <c r="A22" s="30"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -2852,7 +3121,7 @@
       <c r="G22" s="5"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
+      <c r="A23" s="30"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -2861,7 +3130,7 @@
       <c r="G23" s="5"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
+      <c r="A24" s="30"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -2871,7 +3140,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D11">
       <formula1>"Completed,Pending"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>